<commit_message>
ui import from xls done
</commit_message>
<xml_diff>
--- a/Engine/data/ui_parameter.xlsx
+++ b/Engine/data/ui_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F99631-308E-49F3-8783-BC1E432DA81F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E3D000-26D2-44EC-8944-D41947E6FAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
-    <t>UI_COMPONENT_COUNT</t>
+    <t>FILENAME</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
+    <t>POSITION_X</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>How many UI components</t>
+    <t>POSITION_Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor.png</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bullet.png</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE_X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE_Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 원래 사이즈를 사용하고 싶으면 0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -983,29 +1003,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hp ui component moved to uimanagerclass
</commit_message>
<xml_diff>
--- a/Engine/data/ui_parameter.xlsx
+++ b/Engine/data/ui_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E3D000-26D2-44EC-8944-D41947E6FAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AB259D-BF2D-480C-89F2-A36082D88BD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,37 +20,65 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
-  <si>
-    <t>FILENAME</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>POSITION_X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>POSITION_Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>floor.png</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>bullet.png</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SIZE_X</t>
+    <t>이미지 원래 사이즈를 사용하고 싶으면 0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SIZE_Y</t>
+    <t>button.png</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>이미지 원래 사이즈를 사용하고 싶으면 0</t>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position_X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position_Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size_X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size_Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>button1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>button2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>button3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>button4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSSHPBAR_FRONT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSSHPBAR_BACK</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -515,6 +543,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -644,8 +734,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1003,108 +1111,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B33" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
+      <c r="B35" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>200</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>200</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
+    <row r="36" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="6">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
boss hp bar done
</commit_message>
<xml_diff>
--- a/Engine/data/ui_parameter.xlsx
+++ b/Engine/data/ui_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AB259D-BF2D-480C-89F2-A36082D88BD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E47507-FC97-4A10-B208-BD899BE19E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1332,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
boss pattern interface and player hp bar
</commit_message>
<xml_diff>
--- a/Engine/data/ui_parameter.xlsx
+++ b/Engine/data/ui_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E47507-FC97-4A10-B208-BD899BE19E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2F2C6C-0B81-4F7B-AF31-F616F5B77971}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="3945" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="player_parameter" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
   <si>
     <t>bullet.png</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -74,11 +74,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>BOSSHPBAR_FRONT</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSSHPBAR_BACK</t>
+    <t>PLAYER_HPBAR_BACK</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS_HPBAR_FRONT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS_HPBAR_BACK</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYER_HPBAR_FRONT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS HP바의 뒷 이미지</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS HP바의 앞 이미지</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -734,27 +750,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1111,16 +1130,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="26" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1263,7 +1282,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1271,7 +1290,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1298,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1303,7 +1322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -1311,7 +1330,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1319,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1327,15 +1346,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1373,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1389,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
@@ -1375,15 +1397,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1420,6 +1445,102 @@
         <v>8</v>
       </c>
       <c r="B36" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="6">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
player doesn't go out of the map
</commit_message>
<xml_diff>
--- a/Engine/data/ui_parameter.xlsx
+++ b/Engine/data/ui_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2F2C6C-0B81-4F7B-AF31-F616F5B77971}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4734C00-C774-471B-A325-520465EED135}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="3945" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="4">
-        <v>300</v>
+        <v>810</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1386,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1421,7 +1421,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="4">
-        <v>300</v>
+        <v>810</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="4">
-        <v>300</v>
+        <v>810</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1477,7 +1477,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="4">
-        <v>500</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1485,7 +1485,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1517,7 +1517,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="4">
-        <v>300</v>
+        <v>810</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1525,7 +1525,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="4">
-        <v>500</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1533,7 +1533,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>